<commit_message>
add cols to password excel
</commit_message>
<xml_diff>
--- a/workOnExcel/passwarde.xlsx
+++ b/workOnExcel/passwarde.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C078C114-2D11-4E20-B392-7E4B1C14D5FA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t xml:space="preserve">user name </t>
   </si>
@@ -43,16 +44,78 @@
   </si>
   <si>
     <t>worker</t>
+  </si>
+  <si>
+    <t>last name</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>bar</t>
+  </si>
+  <si>
+    <t>tsho</t>
+  </si>
+  <si>
+    <t>zor</t>
+  </si>
+  <si>
+    <t>shir@gmail.com</t>
+  </si>
+  <si>
+    <t>michal@gmail.com</t>
+  </si>
+  <si>
+    <t>emilia@gmail.com</t>
+  </si>
+  <si>
+    <t>tair</t>
+  </si>
+  <si>
+    <t>hadad</t>
+  </si>
+  <si>
+    <t>asaf</t>
+  </si>
+  <si>
+    <t>rdt</t>
+  </si>
+  <si>
+    <t>yoni</t>
+  </si>
+  <si>
+    <t>machluf</t>
+  </si>
+  <si>
+    <t>tair@gmail.com</t>
+  </si>
+  <si>
+    <t>asaf@gmail.com</t>
+  </si>
+  <si>
+    <t>yoni@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,20 +138,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="היפר-קישור" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -137,7 +206,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -170,9 +239,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -205,6 +291,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -380,21 +483,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.3984375" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="22.69921875" customWidth="1"/>
+    <col min="2" max="2" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -404,8 +510,17 @@
       <c r="C1" t="s">
         <v>5</v>
       </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -415,8 +530,17 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>123234345</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -426,8 +550,17 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>234345456</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -435,17 +568,94 @@
         <v>222222</v>
       </c>
       <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>345456567</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>123</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5">
+        <v>111111111</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>123</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>111111112</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>123</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7">
+        <v>111111113</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{C356BEF1-26AF-4C70-A608-8E455D9E44B9}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{57A9A79A-842B-4D15-866C-8F249234568F}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{994CD606-676E-4F88-9FEB-F1647B55F6FC}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{C5BE7160-EFBD-46DE-9F71-6442294B31AC}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{3F510F8F-0863-4876-B8F5-2212BCD05DAF}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{64EA1464-557D-4FDF-A968-B2027EF66627}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0"/>
@@ -457,7 +667,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0"/>

</xml_diff>